<commit_message>
top 3 bottom 3
</commit_message>
<xml_diff>
--- a/src/Berglas.xlsx
+++ b/src/Berglas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24729"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anon\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anon\Desktop\Berglas-master\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71B0791-4D85-42E7-886F-2D485A256737}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B13A61-98F1-422D-A141-052476661883}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7908" yWindow="5556" windowWidth="23040" windowHeight="12312" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -138,9 +138,6 @@
     <t>梅花4</t>
   </si>
   <si>
-    <t>梅花10</t>
-  </si>
-  <si>
     <t>梅花7</t>
   </si>
   <si>
@@ -450,28 +447,6 @@
         <family val="3"/>
         <charset val="134"/>
       </rPr>
-      <t>方片</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>7</t>
-    </r>
-    <phoneticPr fontId="4" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
       <t>黑桃</t>
     </r>
     <r>
@@ -591,6 +566,33 @@
   </si>
   <si>
     <t>面无鬼</t>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>方片</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>7</t>
+    </r>
+    <phoneticPr fontId="4" type="noConversion"/>
+  </si>
+  <si>
+    <t>梅花10</t>
     <phoneticPr fontId="4" type="noConversion"/>
   </si>
 </sst>
@@ -915,13 +917,13 @@
   </sheetPr>
   <dimension ref="A1:AC59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -938,21 +940,21 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -962,9 +964,9 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -974,9 +976,9 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -986,9 +988,9 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B5" s="1">
         <v>1</v>
@@ -1019,7 +1021,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
@@ -1052,7 +1054,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
@@ -1085,7 +1087,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
@@ -1118,7 +1120,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -1151,7 +1153,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
@@ -1184,7 +1186,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
@@ -1217,7 +1219,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
@@ -1250,7 +1252,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
@@ -1283,7 +1285,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
@@ -1316,7 +1318,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
@@ -1382,7 +1384,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
@@ -1415,7 +1417,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
@@ -1448,7 +1450,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
@@ -1481,7 +1483,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -1514,7 +1516,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1547,7 +1549,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
@@ -1580,7 +1582,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
@@ -1613,7 +1615,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
@@ -1646,7 +1648,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
@@ -1679,7 +1681,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
@@ -1712,7 +1714,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
@@ -1745,7 +1747,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
         <v>27</v>
       </c>
@@ -1798,7 +1800,7 @@
       <c r="AB28" s="6"/>
       <c r="AC28" s="6"/>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
@@ -1831,7 +1833,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
@@ -1864,7 +1866,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
         <v>30</v>
       </c>
@@ -1897,7 +1899,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:29" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
         <v>31</v>
       </c>
@@ -1930,7 +1932,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>32</v>
       </c>
@@ -1963,7 +1965,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>33</v>
       </c>
@@ -1996,7 +1998,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
         <v>34</v>
       </c>
@@ -2029,9 +2031,9 @@
         <v>24</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A36" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B36" s="1">
         <v>32</v>
@@ -2062,9 +2064,9 @@
         <v>23</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>35</v>
+    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A37" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="B37" s="1">
         <v>33</v>
@@ -2095,9 +2097,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1">
         <v>34</v>
@@ -2128,9 +2130,9 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1">
         <v>35</v>
@@ -2161,9 +2163,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B40" s="1">
         <v>36</v>
@@ -2194,9 +2196,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B41" s="1">
         <v>37</v>
@@ -2227,9 +2229,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" s="1">
         <v>38</v>
@@ -2260,9 +2262,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" s="1">
         <v>39</v>
@@ -2293,9 +2295,9 @@
         <v>16</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" s="1">
         <v>40</v>
@@ -2326,9 +2328,9 @@
         <v>15</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" s="1">
         <v>41</v>
@@ -2359,9 +2361,9 @@
         <v>14</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" s="1">
         <v>42</v>
@@ -2392,9 +2394,9 @@
         <v>13</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A47" s="7" t="s">
-        <v>46</v>
+    <row r="47" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A47" s="11" t="s">
+        <v>64</v>
       </c>
       <c r="B47" s="1">
         <v>43</v>
@@ -2425,9 +2427,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
-        <v>47</v>
+        <v>63</v>
       </c>
       <c r="B48" s="1">
         <v>44</v>
@@ -2458,9 +2460,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B49" s="1">
         <v>45</v>
@@ -2491,12 +2493,12 @@
         <v>10</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B50" s="1">
         <v>46</v>
@@ -2527,9 +2529,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B51" s="1">
         <v>47</v>
@@ -2560,9 +2562,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B52" s="1">
         <v>48</v>
@@ -2592,9 +2594,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B53" s="1">
         <v>49</v>
@@ -2624,9 +2626,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="B54" s="1">
         <v>50</v>
@@ -2656,9 +2658,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B55" s="1">
         <v>51</v>
@@ -2688,9 +2690,9 @@
         <v>4</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B56" s="1">
         <v>52</v>
@@ -2722,17 +2724,17 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -2755,7 +2757,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2772,21 +2774,21 @@
         <v>4</v>
       </c>
       <c r="F1" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="G1" s="7" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A2" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -2796,9 +2798,9 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -2808,9 +2810,9 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -4239,7 +4241,7 @@
         <v>10</v>
       </c>
       <c r="L49" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:12" ht="13.2" x14ac:dyDescent="0.25">
@@ -4456,17 +4458,17 @@
     </row>
     <row r="57" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="10" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="58" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="10" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="59" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="10" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>